<commit_message>
Moved all files used for the consequence table number predications for the May 2024 workshop into the CWD_model_Cross folder
</commit_message>
<xml_diff>
--- a/CWD_model_Cross/data/NE_Deer_Params_litreview.xlsx
+++ b/CWD_model_Cross/data/NE_Deer_Params_litreview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uvmoffice-my.sharepoint.com/personal/astanle1_uvm_edu/Documents/Documents/VTCWD/CWD_model_Cross/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uvmoffice-my.sharepoint.com/personal/astanle1_uvm_edu/Documents/Documents/VTCWD/CWD_model_Cross/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1F68471-440F-40E8-AFF6-881973B1FB3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{F1F68471-440F-40E8-AFF6-881973B1FB3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CAC7777-4950-4FB5-BC85-6D260D7A546C}"/>
   <bookViews>
-    <workbookView xWindow="490" yWindow="220" windowWidth="19180" windowHeight="10170" xr2:uid="{76CABE02-8CD5-4E0B-AF7A-35B6BFCC6C93}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{76CABE02-8CD5-4E0B-AF7A-35B6BFCC6C93}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="64">
   <si>
     <t>Parameter</t>
   </si>
@@ -188,9 +188,6 @@
     <t>https://www.proquest.com/openview/4b4191a6892187d49b725aa92b049787/1?pq-origsite=gscholar&amp;cbl=18750</t>
   </si>
   <si>
-    <t>XX</t>
-  </si>
-  <si>
     <t>https://www.jstor.org/stable/pdf/3802199.pdf</t>
   </si>
   <si>
@@ -222,6 +219,15 @@
   </si>
   <si>
     <t>Nick spreadshet</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>VT spreadsheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -613,7 +619,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -649,6 +655,12 @@
       <c r="J1" t="s">
         <v>33</v>
       </c>
+      <c r="L1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -664,9 +676,6 @@
       <c r="F2">
         <v>0.6</v>
       </c>
-      <c r="K2" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -679,7 +688,7 @@
         <v>0.8</v>
       </c>
       <c r="L3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -693,7 +702,7 @@
         <v>0.95</v>
       </c>
       <c r="L4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -704,7 +713,7 @@
         <v>0.9</v>
       </c>
       <c r="L5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -752,7 +761,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -882,7 +891,7 @@
         <v>28</v>
       </c>
       <c r="E18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G18" t="s">
         <v>29</v>
@@ -900,10 +909,10 @@
         <v>49</v>
       </c>
       <c r="L18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
@@ -911,16 +920,28 @@
         <v>4</v>
       </c>
       <c r="G20" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="H20" t="s">
+        <v>55</v>
+      </c>
+      <c r="I20" t="s">
+        <v>55</v>
+      </c>
+      <c r="J20" t="s">
+        <v>55</v>
+      </c>
+      <c r="K20" t="s">
+        <v>63</v>
       </c>
       <c r="L20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M20" t="s">
+        <v>57</v>
+      </c>
+      <c r="N20" t="s">
         <v>58</v>
-      </c>
-      <c r="N20" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>